<commit_message>
Feat: Random bug fix
</commit_message>
<xml_diff>
--- a/public/import/import-meja.xlsx
+++ b/public/import/import-meja.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Sandisk 16gb\Kelas XII\Vemto\Test\File for import data on KZ_Coffee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Sandisk 16gb\Kelas XII\Vemto\Test\kz_coffee\public\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DDFB89-42DE-4FE6-AFF9-1706A4D6EA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DFDAAA-FD73-465B-BC9E-8179EA018C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6192" yWindow="1344" windowWidth="14952" windowHeight="9900" xr2:uid="{FB9D911A-E180-4CC6-BD5C-CC0466ADB06C}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="14952" windowHeight="9900" xr2:uid="{FB9D911A-E180-4CC6-BD5C-CC0466ADB06C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
   <si>
     <t>Nomor Meja</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>tersedia</t>
-  </si>
-  <si>
-    <t>terpakai</t>
   </si>
 </sst>
 </file>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22CFCB9-AEAD-4470-A337-5E719137593B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +437,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
@@ -451,7 +448,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -462,7 +459,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>5</v>
@@ -473,7 +470,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -484,7 +481,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -495,7 +492,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -506,24 +503,57 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>